<commit_message>
Cambio de formato para documento de aulas por defecto. Ahora, la primera columna sera el nombre del aula
</commit_message>
<xml_diff>
--- a/src/asignacion_aulica/data/aulas.xlsx
+++ b/src/asignacion_aulica/data/aulas.xlsx
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">edificio </t>
-  </si>
-  <si>
     <t xml:space="preserve">nombre </t>
   </si>
   <si>
@@ -39,6 +36,9 @@
   <si>
     <t xml:space="preserve">horario_cierre </t>
   </si>
+  <si>
+    <t xml:space="preserve">edificio</t>
+  </si>
 </sst>
 </file>
 
@@ -52,6 +52,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -72,6 +73,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,13 +118,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -142,10 +148,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -166,9 +172,12 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Agregado de casos de prueba en aula.xlsx , y implementacion incompleta de insertar aulas en universidad.py
</commit_message>
<xml_diff>
--- a/src/asignacion_aulica/data/aulas.xlsx
+++ b/src/asignacion_aulica/data/aulas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">nombre </t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t xml:space="preserve">edificio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“proyector, computadoras”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anasagasti 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“proyector”</t>
   </si>
 </sst>
 </file>
@@ -47,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -73,6 +88,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -118,7 +140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -127,7 +149,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -148,13 +174,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.76"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -172,12 +203,37 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>